<commit_message>
update, tissā, uposatha days
</commit_message>
<xml_diff>
--- a/docs/DPD Add Words.xlsx
+++ b/docs/DPD Add Words.xlsx
@@ -84,7 +84,7 @@
     <t xml:space="preserve">sabba + ratti</t>
   </si>
   <si>
-    <t xml:space="preserve">atha kho yasassa kulaputtassa pañcahi kāmaguṇehi samappitassa samaṅgībhūtassa paricārayamānassa paṭikacc'eva niddā okkami, parijanassapi niddā okkami, sabbarattiyo ca telapadīpo jhāyati.</t>
+    <t xml:space="preserve">atha kho yasassa kulaputtassa pañcahi kāmaguṇehi samappitassa samaṅgībhūtassa paricārayamānassa paṭikacceva niddā okkami, parijanassapi niddā okkami, sabbarattiyo ca telapadīpo jhāyati.</t>
   </si>
   <si>
     <t xml:space="preserve">vinaya, mahāvagga</t>
@@ -693,7 +693,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -726,8 +726,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -768,7 +772,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -910,7 +914,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>1</v>
       </c>
@@ -931,7 +935,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>2</v>
       </c>
@@ -952,7 +956,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>3</v>
       </c>
@@ -973,7 +977,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>4</v>
       </c>
@@ -994,7 +998,7 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>5</v>
       </c>
@@ -1015,7 +1019,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>6</v>
       </c>
@@ -1036,7 +1040,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>7</v>
       </c>
@@ -1057,7 +1061,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>8</v>
       </c>
@@ -1078,7 +1082,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>9</v>
       </c>
@@ -1099,7 +1103,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>10</v>
       </c>
@@ -1122,7 +1126,7 @@
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
-      <c r="B16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1173,42 +1177,42 @@
       <c r="Q17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="3"/>
@@ -1216,20 +1220,20 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="3"/>
@@ -1250,7 +1254,7 @@
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="3"/>
@@ -1271,7 +1275,7 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="3"/>
@@ -1292,7 +1296,7 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="3"/>
@@ -1313,7 +1317,7 @@
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="12" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="3"/>
@@ -1334,7 +1338,7 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="3"/>
@@ -1355,7 +1359,7 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="3"/>
@@ -1376,7 +1380,7 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D27" s="3"/>
@@ -1397,7 +1401,7 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D28" s="3"/>
@@ -1418,7 +1422,7 @@
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="3"/>
@@ -1439,7 +1443,7 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="3"/>
@@ -1460,7 +1464,7 @@
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="3"/>
@@ -1481,7 +1485,7 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D32" s="3"/>
@@ -1502,7 +1506,7 @@
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D33" s="3"/>
@@ -1523,7 +1527,7 @@
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D34" s="3"/>
@@ -1544,7 +1548,7 @@
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D35" s="3"/>
@@ -1565,7 +1569,7 @@
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="12" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="3"/>
@@ -1586,7 +1590,7 @@
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D37" s="3"/>
@@ -1607,7 +1611,7 @@
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D38" s="3"/>
@@ -1628,7 +1632,7 @@
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D39" s="3"/>
@@ -1649,7 +1653,7 @@
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D40" s="3"/>
@@ -1670,7 +1674,7 @@
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="3"/>
@@ -1691,7 +1695,7 @@
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="12" t="s">
         <v>47</v>
       </c>
       <c r="D42" s="3"/>
@@ -1712,7 +1716,7 @@
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D43" s="3"/>
@@ -1733,7 +1737,7 @@
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D44" s="3"/>
@@ -1754,7 +1758,7 @@
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="12" t="s">
         <v>50</v>
       </c>
       <c r="D45" s="3"/>
@@ -1775,7 +1779,7 @@
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D46" s="3"/>

</xml_diff>